<commit_message>
[110]-Update nhan dien thuong hieu - Cuong
</commit_message>
<xml_diff>
--- a/assets/public/csv/export/Devices.xlsx
+++ b/assets/public/csv/export/Devices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
   <si>
     <t>ĐẠI HỌC HUẾ</t>
   </si>
@@ -118,7 +118,13 @@
     <t>Bàn học sinh ván MDF 1.2m*0.75m</t>
   </si>
   <si>
-    <t>Nam Cuong</t>
+    <t>Quạt Senko xuất xứ ASIAN</t>
+  </si>
+  <si>
+    <t>Máy in lazer HP Pro M404Dn</t>
+  </si>
+  <si>
+    <t>Switch D link 16 port 1000Mb</t>
   </si>
 </sst>
 </file>
@@ -578,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="G16" sqref="G16"/>
@@ -1218,33 +1224,115 @@
         <v>28</v>
       </c>
       <c r="D24">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>4800000</v>
+      </c>
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>4800000</v>
+      </c>
+      <c r="J24" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>4800000</v>
+      </c>
+      <c r="M24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25">
+        <v>2019</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>6996000</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>6996000</v>
+      </c>
+      <c r="J25" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>6996000</v>
+      </c>
+      <c r="M25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26">
+        <v>2019</v>
+      </c>
+      <c r="E26">
         <v>2</v>
       </c>
-      <c r="F24">
-        <v>2000</v>
-      </c>
-      <c r="G24" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24">
+      <c r="F26">
+        <v>10240000</v>
+      </c>
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26">
         <v>2</v>
       </c>
-      <c r="I24">
-        <v>2000</v>
-      </c>
-      <c r="J24" t="s">
-        <v>28</v>
-      </c>
-      <c r="K24">
+      <c r="I26">
+        <v>10240000</v>
+      </c>
+      <c r="J26" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26">
         <v>2</v>
       </c>
-      <c r="L24">
-        <v>2000</v>
-      </c>
-      <c r="M24" t="s">
+      <c r="L26">
+        <v>10240000</v>
+      </c>
+      <c r="M26" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>